<commit_message>
add dual port digital qpsk modulator
</commit_message>
<xml_diff>
--- a/doc/sm_tables.xlsx
+++ b/doc/sm_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prj\legendary-octo-barnacle\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B51927-300C-4D43-99B0-05DB35EEEAC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C261E3C6-26A3-4C97-A60C-231A28BB46A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="852" windowWidth="20424" windowHeight="11100" xr2:uid="{A4492641-E264-49F8-BEB0-D2D1BAB2691E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A4492641-E264-49F8-BEB0-D2D1BAB2691E}"/>
   </bookViews>
   <sheets>
     <sheet name="selector" sheetId="3" r:id="rId1"/>
@@ -748,70 +748,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
@@ -826,73 +823,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
@@ -901,7 +892,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1247,64 +1247,64 @@
     </row>
     <row r="2" spans="1:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="33" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
       <c r="J2" s="13" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="43" t="s">
         <v>13</v>
       </c>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="46"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="44"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
@@ -1369,244 +1369,244 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
-      <c r="B7" s="26">
-        <v>0</v>
-      </c>
-      <c r="C7" s="28">
+      <c r="B7" s="45">
+        <v>0</v>
+      </c>
+      <c r="C7" s="48">
         <v>1</v>
       </c>
       <c r="D7" s="14">
         <v>1</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="51">
         <v>1</v>
       </c>
-      <c r="F7" s="24">
-        <v>0</v>
-      </c>
-      <c r="G7" s="26">
+      <c r="F7" s="53">
+        <v>0</v>
+      </c>
+      <c r="G7" s="45">
         <v>1</v>
       </c>
-      <c r="H7" s="18">
-        <v>0</v>
-      </c>
-      <c r="I7" s="21">
+      <c r="H7" s="56">
+        <v>0</v>
+      </c>
+      <c r="I7" s="51">
         <v>1</v>
       </c>
-      <c r="J7" s="24" t="s">
+      <c r="J7" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="55"/>
-      <c r="L7" s="61" t="s">
+      <c r="K7" s="21"/>
+      <c r="L7" s="60" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="29"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="49"/>
       <c r="D8" s="14">
         <v>0</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="61"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="60"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="29"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="49"/>
       <c r="D9" s="14">
         <v>1</v>
       </c>
-      <c r="E9" s="21">
-        <v>0</v>
-      </c>
-      <c r="F9" s="31"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="24" t="s">
+      <c r="E9" s="51">
+        <v>0</v>
+      </c>
+      <c r="F9" s="54"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="57"/>
-      <c r="L9" s="61"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="60"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="29"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="49"/>
       <c r="D10" s="15">
         <v>0</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="61"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="60"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="29"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="14">
         <v>1</v>
       </c>
-      <c r="E11" s="21">
-        <v>0</v>
-      </c>
-      <c r="F11" s="24">
+      <c r="E11" s="51">
+        <v>0</v>
+      </c>
+      <c r="F11" s="53">
         <v>1</v>
       </c>
-      <c r="G11" s="27"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="61"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="60"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="29"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="49"/>
       <c r="D12" s="14">
         <v>0</v>
       </c>
-      <c r="E12" s="23"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="18">
+      <c r="E12" s="52"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="56">
         <v>1</v>
       </c>
-      <c r="I12" s="23"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="61"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="60"/>
       <c r="O12" s="17"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="29"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="49"/>
       <c r="D13" s="14">
         <v>0</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="51">
         <v>1</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="19"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="57"/>
       <c r="I13" s="16">
         <v>0</v>
       </c>
-      <c r="J13" s="25"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="61"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="60"/>
     </row>
     <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="47">
+      <c r="B14" s="47"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="18">
         <v>1</v>
       </c>
-      <c r="E14" s="53"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="48">
+      <c r="E14" s="63"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="19">
         <v>1</v>
       </c>
-      <c r="J14" s="49">
-        <v>0</v>
-      </c>
-      <c r="K14" s="59"/>
-      <c r="L14" s="61"/>
+      <c r="J14" s="20">
+        <v>0</v>
+      </c>
+      <c r="K14" s="25"/>
+      <c r="L14" s="60"/>
     </row>
     <row r="15" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="62"/>
+      <c r="L15" s="27"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="64"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="67"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="68"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="65"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="64"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="66"/>
-      <c r="J17" s="69"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="68"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="64"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="66"/>
-      <c r="I18" s="66"/>
-      <c r="J18" s="69"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="68"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="64"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="66"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="66"/>
-      <c r="G19" s="66"/>
-      <c r="H19" s="66"/>
-      <c r="I19" s="66"/>
-      <c r="J19" s="69"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="68"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="64"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="65"/>
-      <c r="I20" s="65"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="66"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="69"/>
       <c r="J20" s="70"/>
     </row>
   </sheetData>
@@ -1644,6 +1644,7 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>